<commit_message>
added frontend accesscontrol for replies
</commit_message>
<xml_diff>
--- a/database structure.xlsx
+++ b/database structure.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theti\Documents\ECS153FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731EA88B-1CDC-4692-9CC6-376FEC27435F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3AC18A-42E0-40F8-A02F-A4568E8CF9A2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{96A1CB14-85F7-4201-AA76-7B730BB10867}"/>
-    <workbookView xWindow="6548" yWindow="450" windowWidth="22514" windowHeight="14415" xr2:uid="{BBA2D72A-4435-4248-97CA-6B44CABF8396}"/>
+    <workbookView xWindow="5835" yWindow="1260" windowWidth="22695" windowHeight="14595" xr2:uid="{96A1CB14-85F7-4201-AA76-7B730BB10867}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="3" xr2:uid="{BBA2D72A-4435-4248-97CA-6B44CABF8396}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3 (2)" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="84">
   <si>
     <t>username</t>
   </si>
@@ -216,13 +218,82 @@
   </si>
   <si>
     <t>roles is for internal use only</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Guest</t>
+  </si>
+  <si>
+    <t>READ</t>
+  </si>
+  <si>
+    <t>public categories</t>
+  </si>
+  <si>
+    <t>CREATE</t>
+  </si>
+  <si>
+    <t>post/reply in public category</t>
+  </si>
+  <si>
+    <t>UPDATE</t>
+  </si>
+  <si>
+    <t>owned post</t>
+  </si>
+  <si>
+    <t>owned reply</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>post/reply in member category</t>
+  </si>
+  <si>
+    <t>member categories</t>
+  </si>
+  <si>
+    <t>Owner (member of category)</t>
+  </si>
+  <si>
+    <t>Moderator (member of category)</t>
+  </si>
+  <si>
+    <t>Admin (member of all categories)</t>
+  </si>
+  <si>
+    <t>add user to member category</t>
+  </si>
+  <si>
+    <t>add moderator to member category</t>
+  </si>
+  <si>
+    <t>user from member category</t>
+  </si>
+  <si>
+    <t>member category</t>
+  </si>
+  <si>
+    <t>moderator from member category</t>
+  </si>
+  <si>
+    <t>name of member category</t>
+  </si>
+  <si>
+    <t>visibility of member category</t>
+  </si>
+  <si>
+    <t>owner of category</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,6 +305,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -265,7 +343,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -390,11 +468,117 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -486,6 +670,59 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -803,10 +1040,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{761E0DC3-F663-4E2D-AB35-A11283046FA4}">
   <dimension ref="B2:AC37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="AD39" sqref="AD39"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
+    <sheetView workbookViewId="1">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1922,4 +2159,1223 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327440FF-2854-4412-BA2F-3A5ADA2F32F0}">
+  <dimension ref="B4:P31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="93" workbookViewId="1">
+      <selection sqref="A1:R39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="3" width="3.06640625" customWidth="1"/>
+    <col min="4" max="4" width="28.73046875" customWidth="1"/>
+    <col min="5" max="6" width="3.06640625" customWidth="1"/>
+    <col min="7" max="7" width="28.73046875" customWidth="1"/>
+    <col min="8" max="9" width="3.06640625" customWidth="1"/>
+    <col min="10" max="10" width="28.73046875" customWidth="1"/>
+    <col min="11" max="12" width="3.06640625" customWidth="1"/>
+    <col min="13" max="13" width="28.73046875" customWidth="1"/>
+    <col min="14" max="15" width="3.06640625" customWidth="1"/>
+    <col min="16" max="16" width="28.73046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L4" t="s">
+        <v>61</v>
+      </c>
+      <c r="O4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B6" s="32"/>
+      <c r="C6" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="P6" s="34"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B7" s="35"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="37" t="str">
+        <f>G7</f>
+        <v>public categories</v>
+      </c>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="37" t="str">
+        <f>J7</f>
+        <v>public categories</v>
+      </c>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="37" t="str">
+        <f>M7</f>
+        <v>public categories</v>
+      </c>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="37" t="str">
+        <f>P7</f>
+        <v>public categories</v>
+      </c>
+      <c r="N7" s="36"/>
+      <c r="O7" s="36"/>
+      <c r="P7" s="38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B8" s="35"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="37" t="str">
+        <f>G8</f>
+        <v>member categories</v>
+      </c>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="37" t="str">
+        <f>J8</f>
+        <v>member categories</v>
+      </c>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="37" t="str">
+        <f>M8</f>
+        <v>member categories</v>
+      </c>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="N8" s="36"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="38"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B9" s="39"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="41"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B11" s="32"/>
+      <c r="C11" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
+      <c r="O11" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="P11" s="34"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B12" s="35"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="37" t="str">
+        <f>G12</f>
+        <v>category</v>
+      </c>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="37" t="str">
+        <f>J12</f>
+        <v>category</v>
+      </c>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="37" t="str">
+        <f>M12</f>
+        <v>category</v>
+      </c>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="38"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B13" s="35"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="37" t="str">
+        <f>G13</f>
+        <v>post/reply in public category</v>
+      </c>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="37" t="str">
+        <f>J13</f>
+        <v>post/reply in public category</v>
+      </c>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="37" t="str">
+        <f>M13</f>
+        <v>post/reply in public category</v>
+      </c>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="N13" s="36"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="38"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B14" s="35"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="37" t="str">
+        <f>G14</f>
+        <v>post/reply in member category</v>
+      </c>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="37" t="str">
+        <f>J14</f>
+        <v>post/reply in member category</v>
+      </c>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="37" t="str">
+        <f>M14</f>
+        <v>post/reply in member category</v>
+      </c>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="N14" s="36"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="38"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B15" s="35"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="37" t="str">
+        <f>G15</f>
+        <v>add user to member category</v>
+      </c>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="37" t="str">
+        <f>J15</f>
+        <v>add user to member category</v>
+      </c>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="38"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B16" s="39"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="42" t="str">
+        <f>G16</f>
+        <v>add moderator to member category</v>
+      </c>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="40"/>
+      <c r="P16" s="41"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B18" s="43"/>
+      <c r="C18" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="M18" s="33"/>
+      <c r="N18" s="33"/>
+      <c r="O18" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="P18" s="34"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B19" s="44"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="37" t="str">
+        <f>M19</f>
+        <v>owned post</v>
+      </c>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="37" t="str">
+        <f>M19</f>
+        <v>owned post</v>
+      </c>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="37" t="str">
+        <f>M19</f>
+        <v>owned post</v>
+      </c>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="N19" s="36"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="38"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B20" s="44"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="37" t="str">
+        <f>M20</f>
+        <v>owned reply</v>
+      </c>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="37" t="str">
+        <f>M20</f>
+        <v>owned reply</v>
+      </c>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="37" t="str">
+        <f>M20</f>
+        <v>owned reply</v>
+      </c>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="N20" s="36"/>
+      <c r="O20" s="36"/>
+      <c r="P20" s="38"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B21" s="44"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="37" t="str">
+        <f>G21</f>
+        <v>name of member category</v>
+      </c>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="36"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="38"/>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B22" s="44"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="37" t="str">
+        <f>G22</f>
+        <v>visibility of member category</v>
+      </c>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="36"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="38"/>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B23" s="45"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="40"/>
+      <c r="O23" s="40"/>
+      <c r="P23" s="41"/>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B25" s="32"/>
+      <c r="C25" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="P25" s="34"/>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B26" s="35"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="37" t="str">
+        <f>M26</f>
+        <v>owned post</v>
+      </c>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="37" t="str">
+        <f>M26</f>
+        <v>owned post</v>
+      </c>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="37" t="str">
+        <f>M26</f>
+        <v>owned post</v>
+      </c>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="N26" s="36"/>
+      <c r="O26" s="36"/>
+      <c r="P26" s="38"/>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B27" s="35"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="37" t="str">
+        <f>M27</f>
+        <v>owned reply</v>
+      </c>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="37" t="str">
+        <f>M27</f>
+        <v>owned reply</v>
+      </c>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="37" t="str">
+        <f>M27</f>
+        <v>owned reply</v>
+      </c>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="N27" s="36"/>
+      <c r="O27" s="36"/>
+      <c r="P27" s="38"/>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B28" s="35"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="37" t="str">
+        <f>J28</f>
+        <v>user from member category</v>
+      </c>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="37" t="str">
+        <f>J28</f>
+        <v>user from member category</v>
+      </c>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="K28" s="36"/>
+      <c r="L28" s="36"/>
+      <c r="M28" s="36"/>
+      <c r="N28" s="36"/>
+      <c r="O28" s="36"/>
+      <c r="P28" s="38"/>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B29" s="35"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="37" t="str">
+        <f>J29</f>
+        <v>post/reply in member category</v>
+      </c>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="37" t="str">
+        <f>J29</f>
+        <v>post/reply in member category</v>
+      </c>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="K29" s="36"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="36"/>
+      <c r="N29" s="36"/>
+      <c r="O29" s="36"/>
+      <c r="P29" s="38"/>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B30" s="35"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="37" t="str">
+        <f>G30</f>
+        <v>member category</v>
+      </c>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="36"/>
+      <c r="M30" s="36"/>
+      <c r="N30" s="36"/>
+      <c r="O30" s="36"/>
+      <c r="P30" s="38"/>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B31" s="39"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="42" t="str">
+        <f>G31</f>
+        <v>moderator from member category</v>
+      </c>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="40"/>
+      <c r="L31" s="40"/>
+      <c r="M31" s="40"/>
+      <c r="N31" s="40"/>
+      <c r="O31" s="40"/>
+      <c r="P31" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B18:B23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFA3AFBD-7A8F-48E1-8700-DD4EFA36B413}">
+  <dimension ref="B4:R27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="99" workbookViewId="1">
+      <selection activeCell="L35" sqref="L35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="3.59765625" style="36" customWidth="1"/>
+    <col min="2" max="4" width="3.06640625" style="36" customWidth="1"/>
+    <col min="5" max="5" width="30.265625" style="36" customWidth="1"/>
+    <col min="6" max="7" width="3.06640625" style="36" customWidth="1"/>
+    <col min="8" max="8" width="30.265625" style="36" customWidth="1"/>
+    <col min="9" max="10" width="3.06640625" style="36" customWidth="1"/>
+    <col min="11" max="11" width="30.265625" style="36" customWidth="1"/>
+    <col min="12" max="13" width="3.06640625" style="36" customWidth="1"/>
+    <col min="14" max="14" width="30.265625" style="36" customWidth="1"/>
+    <col min="15" max="16" width="3.06640625" style="36" customWidth="1"/>
+    <col min="17" max="17" width="30.265625" style="36" customWidth="1"/>
+    <col min="18" max="18" width="3.06640625" style="36" customWidth="1"/>
+    <col min="19" max="16384" width="9.06640625" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="D4" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="56"/>
+      <c r="G4" s="55" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="56"/>
+      <c r="J4" s="57" t="s">
+        <v>74</v>
+      </c>
+      <c r="K4" s="58"/>
+      <c r="M4" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="N4" s="58"/>
+      <c r="P4" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q4" s="58"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="D5" s="35"/>
+      <c r="E5" s="38"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="38"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="38"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="38"/>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="38"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B6" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="49"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="46" t="str">
+        <f>H6</f>
+        <v>public categories</v>
+      </c>
+      <c r="F6" s="33"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="46" t="str">
+        <f>K6</f>
+        <v>public categories</v>
+      </c>
+      <c r="I6" s="33"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="46" t="str">
+        <f>N6</f>
+        <v>public categories</v>
+      </c>
+      <c r="L6" s="33"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="46" t="str">
+        <f>Q6</f>
+        <v>public categories</v>
+      </c>
+      <c r="O6" s="33"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="R6" s="34"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B7" s="54"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="47" t="str">
+        <f>H7</f>
+        <v>member categories</v>
+      </c>
+      <c r="F7" s="40"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="47" t="str">
+        <f>K7</f>
+        <v>member categories</v>
+      </c>
+      <c r="I7" s="40"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="47" t="str">
+        <f>N7</f>
+        <v>member categories</v>
+      </c>
+      <c r="L7" s="40"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="O7" s="40"/>
+      <c r="P7" s="39"/>
+      <c r="Q7" s="41"/>
+      <c r="R7" s="41"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="D8" s="35"/>
+      <c r="E8" s="38"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="38"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="38"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="38"/>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="38"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B9" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="49"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="46" t="str">
+        <f>H9</f>
+        <v>category</v>
+      </c>
+      <c r="F9" s="33"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="46" t="str">
+        <f>K9</f>
+        <v>category</v>
+      </c>
+      <c r="I9" s="33"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="46" t="str">
+        <f>N9</f>
+        <v>category</v>
+      </c>
+      <c r="L9" s="33"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="O9" s="33"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="34"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B10" s="53"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="48" t="str">
+        <f>H10</f>
+        <v>post/reply in public category</v>
+      </c>
+      <c r="G10" s="35"/>
+      <c r="H10" s="48" t="str">
+        <f>K10</f>
+        <v>post/reply in public category</v>
+      </c>
+      <c r="J10" s="35"/>
+      <c r="K10" s="48" t="str">
+        <f>N10</f>
+        <v>post/reply in public category</v>
+      </c>
+      <c r="M10" s="35"/>
+      <c r="N10" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="38"/>
+      <c r="R10" s="38"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B11" s="53"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="48" t="str">
+        <f>H11</f>
+        <v>post/reply in member category</v>
+      </c>
+      <c r="G11" s="35"/>
+      <c r="H11" s="48" t="str">
+        <f>K11</f>
+        <v>post/reply in member category</v>
+      </c>
+      <c r="J11" s="35"/>
+      <c r="K11" s="48" t="str">
+        <f>N11</f>
+        <v>post/reply in member category</v>
+      </c>
+      <c r="M11" s="35"/>
+      <c r="N11" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="P11" s="35"/>
+      <c r="Q11" s="38"/>
+      <c r="R11" s="38"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B12" s="53"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="48" t="str">
+        <f>H12</f>
+        <v>add user to member category</v>
+      </c>
+      <c r="G12" s="35"/>
+      <c r="H12" s="48" t="str">
+        <f>K12</f>
+        <v>add user to member category</v>
+      </c>
+      <c r="J12" s="35"/>
+      <c r="K12" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="M12" s="35"/>
+      <c r="N12" s="38"/>
+      <c r="P12" s="35"/>
+      <c r="Q12" s="38"/>
+      <c r="R12" s="38"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B13" s="54"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="47" t="str">
+        <f>H13</f>
+        <v>add moderator to member category</v>
+      </c>
+      <c r="F13" s="40"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" s="40"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="39"/>
+      <c r="Q13" s="41"/>
+      <c r="R13" s="41"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="D14" s="35"/>
+      <c r="E14" s="38"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="38"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="38"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="38"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="38"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B15" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="49"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="46" t="str">
+        <f>N15</f>
+        <v>owned post</v>
+      </c>
+      <c r="F15" s="33"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="46" t="str">
+        <f>N15</f>
+        <v>owned post</v>
+      </c>
+      <c r="I15" s="33"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="46" t="str">
+        <f>N15</f>
+        <v>owned post</v>
+      </c>
+      <c r="L15" s="33"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="O15" s="33"/>
+      <c r="P15" s="32"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="34"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B16" s="53"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="48" t="str">
+        <f>N16</f>
+        <v>owned reply</v>
+      </c>
+      <c r="G16" s="35"/>
+      <c r="H16" s="48" t="str">
+        <f>N16</f>
+        <v>owned reply</v>
+      </c>
+      <c r="J16" s="35"/>
+      <c r="K16" s="48" t="str">
+        <f>N16</f>
+        <v>owned reply</v>
+      </c>
+      <c r="M16" s="35"/>
+      <c r="N16" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="38"/>
+      <c r="R16" s="38"/>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B17" s="53"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="48" t="str">
+        <f>H17</f>
+        <v>name of member category</v>
+      </c>
+      <c r="G17" s="35"/>
+      <c r="H17" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="J17" s="35"/>
+      <c r="K17" s="38"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="38"/>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="38"/>
+      <c r="R17" s="38"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B18" s="53"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="48" t="str">
+        <f>H18</f>
+        <v>visibility of member category</v>
+      </c>
+      <c r="G18" s="35"/>
+      <c r="H18" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="J18" s="35"/>
+      <c r="K18" s="38"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="38"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="38"/>
+      <c r="R18" s="38"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B19" s="54"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="40"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="41"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="39"/>
+      <c r="Q19" s="41"/>
+      <c r="R19" s="41"/>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="D20" s="35"/>
+      <c r="E20" s="38"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="38"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="38"/>
+      <c r="M20" s="35"/>
+      <c r="N20" s="38"/>
+      <c r="P20" s="35"/>
+      <c r="Q20" s="38"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B21" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="49"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="46" t="str">
+        <f>N21</f>
+        <v>owned post</v>
+      </c>
+      <c r="F21" s="33"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="46" t="str">
+        <f>N21</f>
+        <v>owned post</v>
+      </c>
+      <c r="I21" s="33"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="46" t="str">
+        <f>N21</f>
+        <v>owned post</v>
+      </c>
+      <c r="L21" s="33"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="O21" s="33"/>
+      <c r="P21" s="32"/>
+      <c r="Q21" s="34"/>
+      <c r="R21" s="34"/>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B22" s="53"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="48" t="str">
+        <f>N22</f>
+        <v>owned reply</v>
+      </c>
+      <c r="G22" s="35"/>
+      <c r="H22" s="48" t="str">
+        <f>N22</f>
+        <v>owned reply</v>
+      </c>
+      <c r="J22" s="35"/>
+      <c r="K22" s="48" t="str">
+        <f>N22</f>
+        <v>owned reply</v>
+      </c>
+      <c r="M22" s="35"/>
+      <c r="N22" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="P22" s="35"/>
+      <c r="Q22" s="38"/>
+      <c r="R22" s="38"/>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B23" s="53"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="48" t="str">
+        <f>K23</f>
+        <v>user from member category</v>
+      </c>
+      <c r="G23" s="35"/>
+      <c r="H23" s="48" t="str">
+        <f>K23</f>
+        <v>user from member category</v>
+      </c>
+      <c r="J23" s="35"/>
+      <c r="K23" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="M23" s="35"/>
+      <c r="N23" s="38"/>
+      <c r="P23" s="35"/>
+      <c r="Q23" s="38"/>
+      <c r="R23" s="38"/>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B24" s="53"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="48" t="str">
+        <f>K24</f>
+        <v>post/reply in member category</v>
+      </c>
+      <c r="G24" s="35"/>
+      <c r="H24" s="48" t="str">
+        <f>K24</f>
+        <v>post/reply in member category</v>
+      </c>
+      <c r="J24" s="35"/>
+      <c r="K24" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="M24" s="35"/>
+      <c r="N24" s="38"/>
+      <c r="P24" s="35"/>
+      <c r="Q24" s="38"/>
+      <c r="R24" s="38"/>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B25" s="53"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="48" t="str">
+        <f>H25</f>
+        <v>member category</v>
+      </c>
+      <c r="G25" s="35"/>
+      <c r="H25" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="J25" s="35"/>
+      <c r="K25" s="38"/>
+      <c r="M25" s="35"/>
+      <c r="N25" s="38"/>
+      <c r="P25" s="35"/>
+      <c r="Q25" s="38"/>
+      <c r="R25" s="38"/>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="B26" s="54"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="47" t="str">
+        <f>H26</f>
+        <v>moderator from member category</v>
+      </c>
+      <c r="F26" s="40"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="I26" s="40"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="41"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="39"/>
+      <c r="N26" s="41"/>
+      <c r="O26" s="40"/>
+      <c r="P26" s="39"/>
+      <c r="Q26" s="41"/>
+      <c r="R26" s="41"/>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="D27" s="39"/>
+      <c r="E27" s="41"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="41"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="41"/>
+      <c r="M27" s="39"/>
+      <c r="N27" s="41"/>
+      <c r="P27" s="39"/>
+      <c r="Q27" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="B21:B26"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>